<commit_message>
test results annealing and case results
</commit_message>
<xml_diff>
--- a/CaseResults.xlsx
+++ b/CaseResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="8080" windowWidth="34400" windowHeight="18540" tabRatio="500"/>
+    <workbookView xWindow="7040" yWindow="9840" windowWidth="34400" windowHeight="18620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Lowest Color</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,13 +105,18 @@
   </si>
   <si>
     <t>4.2476580143 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00251889228821 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="14">
+    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="170" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="171" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="173" formatCode="#,##0.00000000000"/>
@@ -120,7 +125,10 @@
     <numFmt numFmtId="177" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="178" formatCode="#,##0.000000000000"/>
     <numFmt numFmtId="179" formatCode="#,##0.00000000000000"/>
+    <numFmt numFmtId="180" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="182" formatCode="#,##0.00000000000000"/>
+    <numFmt numFmtId="184" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="185" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -132,7 +140,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,8 +178,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -186,7 +202,12 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
@@ -519,7 +540,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -529,68 +550,70 @@
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:13" s="8" customFormat="1">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:13" s="8" customFormat="1">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="38" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B3">
@@ -617,20 +640,62 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>6.7223072051999996E-2</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>7.6884984970100004E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="31" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B4" s="18">
+        <v>4</v>
+      </c>
+      <c r="C4" s="18">
+        <v>3.1410932540900001E-2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.106057882309</v>
+      </c>
+      <c r="F4" s="18">
+        <v>5</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>15</v>
+      </c>
+      <c r="H4" s="17">
+        <v>4</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0.13846302032499999</v>
+      </c>
+      <c r="J4" s="17">
+        <v>3</v>
+      </c>
+      <c r="K4" s="17">
+        <v>8.1048965454099994E-2</v>
+      </c>
+      <c r="L4" s="17">
+        <v>3</v>
+      </c>
+      <c r="M4" s="17">
+        <v>8.8603973388700005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -657,85 +722,121 @@
       <c r="I5" t="s">
         <v>21</v>
       </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2.3829936981200001E-3</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="36" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>2.9672808647200002</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="7">
         <v>4.5458459854099997</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="7">
         <v>6.67987895012</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>8.8759930133800005</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" s="13">
+        <v>8.1317451000199998</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" s="13">
+        <v>8.6404919624299996</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="39" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>1.3441350460099999</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>2.00057387352</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="10">
         <v>3.0061280727400002</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="12">
         <v>4.30690908432</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3.2566239833799999</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>3.5883750915500001</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="40" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="11">
         <v>1.1980080604600001</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>2.3753349781000002</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="14">
         <v>3.0136859416999999</v>
       </c>
       <c r="H8">
@@ -743,6 +844,18 @@
       </c>
       <c r="I8" t="s">
         <v>23</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" s="15">
+        <v>8.1179690360999999</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8" s="16">
+        <v>8.2085840702099997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update case results and tests clockwise&lowestcolor
</commit_message>
<xml_diff>
--- a/CaseResults.xlsx
+++ b/CaseResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="9840" windowWidth="34400" windowHeight="18620" tabRatio="500"/>
+    <workbookView xWindow="4860" yWindow="7000" windowWidth="34400" windowHeight="18700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Lowest Color</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,27 +108,26 @@
   </si>
   <si>
     <t xml:space="preserve">0.00251889228821 </t>
+  </si>
+  <si>
+    <t>0.00683689117432 seconds</t>
+  </si>
+  <si>
+    <t>0.00760984420776</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="171" formatCode="#,##0.000000000"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00000000000"/>
-    <numFmt numFmtId="174" formatCode="#,##0.000000000000"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00000000000000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.000000000"/>
-    <numFmt numFmtId="178" formatCode="#,##0.000000000000"/>
-    <numFmt numFmtId="179" formatCode="#,##0.00000000000000"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="182" formatCode="#,##0.00000000000000"/>
-    <numFmt numFmtId="184" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="185" formatCode="#,##0.0000000"/>
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00000000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000000000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00000000000000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -140,7 +139,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +158,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,35 +171,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -540,7 +532,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -657,41 +649,41 @@
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18">
-        <v>4</v>
-      </c>
-      <c r="C4" s="18">
+      <c r="B4" s="17">
+        <v>4</v>
+      </c>
+      <c r="C4" s="17">
         <v>3.1410932540900001E-2</v>
       </c>
-      <c r="D4" s="18">
-        <v>5</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="17">
+        <v>5</v>
+      </c>
+      <c r="E4" s="17">
         <v>0.106057882309</v>
       </c>
-      <c r="F4" s="18">
-        <v>5</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17">
+        <v>5</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="17">
-        <v>4</v>
-      </c>
-      <c r="I4" s="17">
-        <v>0.13846302032499999</v>
+        <v>5</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="J4" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="17">
-        <v>8.1048965454099994E-2</v>
+        <v>9.3941688537599998E-3</v>
       </c>
       <c r="L4" s="17">
-        <v>3</v>
-      </c>
-      <c r="M4" s="17">
-        <v>8.8603973388700005E-2</v>
+        <v>5</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28" customHeight="1">
@@ -849,13 +841,13 @@
         <v>4</v>
       </c>
       <c r="K8" s="15">
-        <v>8.1179690360999999</v>
+        <v>5.9993429184</v>
       </c>
       <c r="L8">
         <v>4</v>
       </c>
       <c r="M8" s="16">
-        <v>8.2085840702099997</v>
+        <v>6.4553999900800001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>